<commit_message>
HAJ-2 :: Role Managment : Validate Add new Role
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -12,14 +12,16 @@
     <sheet name="Driver" sheetId="13" r:id="rId3"/>
     <sheet name="Login" sheetId="66" r:id="rId4"/>
     <sheet name="LoginTest" sheetId="96" r:id="rId5"/>
-    <sheet name="UserManagement" sheetId="81" r:id="rId6"/>
+    <sheet name="UserRoles" sheetId="97" r:id="rId6"/>
+    <sheet name="RoleAuthorities" sheetId="98" r:id="rId7"/>
+    <sheet name="UserManagement" sheetId="81" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Driver!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Driver!$A$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase">Driver!$D$1:$D$1</definedName>
     <definedName name="PartyRole">[1]Sheet1!$B$1:$B$10</definedName>
     <definedName name="PartyRole1">[2]Sheet1!$B$1:$B$10</definedName>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="237">
   <si>
     <t>Execution_Flag</t>
   </si>
@@ -236,9 +238,6 @@
   </si>
   <si>
     <t>InspectionCenter</t>
-  </si>
-  <si>
-    <t>Comments</t>
   </si>
   <si>
     <t>Role</t>
@@ -628,13 +627,145 @@
     <t>1234567898</t>
   </si>
   <si>
-    <t>P@ssw0rd@12</t>
-  </si>
-  <si>
     <t>1-3</t>
   </si>
   <si>
     <t>LoginTest</t>
+  </si>
+  <si>
+    <t>Admin Dashboard</t>
+  </si>
+  <si>
+    <t>Add User</t>
+  </si>
+  <si>
+    <t>Edit User</t>
+  </si>
+  <si>
+    <t>Change User Status</t>
+  </si>
+  <si>
+    <t>Reset Password</t>
+  </si>
+  <si>
+    <t>Delete User</t>
+  </si>
+  <si>
+    <t>Add Role</t>
+  </si>
+  <si>
+    <t>Edit Role</t>
+  </si>
+  <si>
+    <t>Delete Role</t>
+  </si>
+  <si>
+    <t>Change Role Status</t>
+  </si>
+  <si>
+    <t>Reset User Password</t>
+  </si>
+  <si>
+    <t>View Applicant Profile</t>
+  </si>
+  <si>
+    <t>Update Applicant Profile</t>
+  </si>
+  <si>
+    <t>Activate Applicant Card</t>
+  </si>
+  <si>
+    <t>Cancel Applicant Card</t>
+  </si>
+  <si>
+    <t>Suspend Applicant Card</t>
+  </si>
+  <si>
+    <t>Reissue Applicant Card</t>
+  </si>
+  <si>
+    <t>Add Digital ID</t>
+  </si>
+  <si>
+    <t>Add Applicant Profile</t>
+  </si>
+  <si>
+    <t>Approve Applicant Profile</t>
+  </si>
+  <si>
+    <t>View Printing Request Details</t>
+  </si>
+  <si>
+    <t>Add Printing Request</t>
+  </si>
+  <si>
+    <t>Manage Requests</t>
+  </si>
+  <si>
+    <t>View Request Details</t>
+  </si>
+  <si>
+    <t>Create New Request</t>
+  </si>
+  <si>
+    <t>View My Profile</t>
+  </si>
+  <si>
+    <t>Update My Profile</t>
+  </si>
+  <si>
+    <t>Register Hamlah</t>
+  </si>
+  <si>
+    <t>Enquiry Hamlah Registration</t>
+  </si>
+  <si>
+    <t>Validate add new User Role</t>
+  </si>
+  <si>
+    <t>RoleArbName</t>
+  </si>
+  <si>
+    <t>RoleEngName</t>
+  </si>
+  <si>
+    <t>RoleAuthorities</t>
+  </si>
+  <si>
+    <t>TestRole</t>
+  </si>
+  <si>
+    <t>دور إختبار</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>ValidateAddUserRole</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>UserRoleActive</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>AuthorityName</t>
+  </si>
+  <si>
+    <t>Scenario_01</t>
+  </si>
+  <si>
+    <t>1,2</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +1192,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1141,9 +1272,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
@@ -1229,13 +1357,123 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="133">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2837,346 +3075,346 @@
     <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="39" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="38" customWidth="1"/>
     <col min="10" max="10" width="36" customWidth="1"/>
-    <col min="11" max="12" width="36" style="43" customWidth="1"/>
+    <col min="11" max="12" width="36" style="42" customWidth="1"/>
     <col min="13" max="13" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H1" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="38" t="s">
         <v>60</v>
       </c>
       <c r="I1" t="s">
         <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>148</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>166</v>
-      </c>
-      <c r="L1" s="43" t="s">
-        <v>169</v>
+        <v>147</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>168</v>
       </c>
       <c r="M1" t="s">
+        <v>159</v>
+      </c>
+      <c r="N1" t="s">
         <v>160</v>
-      </c>
-      <c r="N1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>147</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>88</v>
+        <v>146</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
-      </c>
-      <c r="H2" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="38" t="s">
         <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="N2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>134</v>
+        <v>120</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>133</v>
       </c>
       <c r="I3" t="s">
         <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>150</v>
-      </c>
-      <c r="K3" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="L3" s="43" t="s">
-        <v>170</v>
+        <v>149</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>169</v>
       </c>
       <c r="M3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="N3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>132</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>135</v>
+        <v>131</v>
+      </c>
+      <c r="H4" s="38" t="s">
+        <v>134</v>
       </c>
       <c r="I4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K4" s="43" t="s">
         <v>150</v>
       </c>
-      <c r="L4" s="43" t="s">
-        <v>171</v>
+      <c r="K4" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>170</v>
       </c>
       <c r="M4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G5" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="39" t="s">
-        <v>136</v>
+      <c r="H5" s="38" t="s">
+        <v>135</v>
       </c>
       <c r="I5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J5" t="s">
-        <v>152</v>
-      </c>
-      <c r="K5" s="43" t="s">
         <v>151</v>
       </c>
-      <c r="L5" s="43" t="s">
-        <v>172</v>
+      <c r="K5" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>171</v>
       </c>
       <c r="M5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="N5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H6" s="39" t="s">
-        <v>137</v>
+        <v>121</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>136</v>
       </c>
       <c r="I6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J6" t="s">
-        <v>153</v>
-      </c>
-      <c r="K6" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="L6" s="43" t="s">
-        <v>75</v>
+      <c r="K6" s="42" t="s">
+        <v>151</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>74</v>
       </c>
       <c r="M6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J7" t="s">
-        <v>154</v>
-      </c>
-      <c r="K7" s="43" t="s">
         <v>153</v>
+      </c>
+      <c r="K7" s="42" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J8" t="s">
-        <v>75</v>
-      </c>
-      <c r="K8" s="43" t="s">
-        <v>168</v>
+        <v>74</v>
+      </c>
+      <c r="K8" s="42" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J9" t="s">
-        <v>155</v>
-      </c>
-      <c r="K9" s="43" t="s">
-        <v>75</v>
+        <v>154</v>
+      </c>
+      <c r="K9" s="42" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3203,7 +3441,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51"/>
+      <c r="A1" s="50"/>
       <c r="B1" s="16" t="s">
         <v>8</v>
       </c>
@@ -3212,16 +3450,16 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
+      <c r="A2" s="51"/>
       <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
@@ -3230,34 +3468,34 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>176</v>
+      <c r="C6" s="46" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
@@ -3266,272 +3504,272 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51"/>
+      <c r="B9" s="14" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="14" t="s">
+      <c r="C9" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="C9" s="7" t="s">
+    </row>
+    <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="14" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="14" t="s">
-        <v>180</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D11" s="45"/>
+        <v>178</v>
+      </c>
+      <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="44"/>
+    </row>
+    <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="51"/>
+      <c r="B13" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="49"/>
+      <c r="D13" s="44"/>
+      <c r="H13" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
+      <c r="M13" s="53"/>
+      <c r="N13" s="53"/>
+      <c r="O13" s="54"/>
+    </row>
+    <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="56"/>
+      <c r="M14" s="56"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="57"/>
+    </row>
+    <row r="15" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
+      <c r="B15" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="49"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="56"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="56"/>
+      <c r="O15" s="57"/>
+    </row>
+    <row r="16" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
+      <c r="B16" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="H16" s="55"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="56"/>
+      <c r="M16" s="56"/>
+      <c r="N16" s="56"/>
+      <c r="O16" s="57"/>
+    </row>
+    <row r="17" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
+      <c r="B17" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="55"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="56"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="56"/>
+      <c r="O17" s="57"/>
+    </row>
+    <row r="18" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
+      <c r="B18" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="D12" s="45"/>
-    </row>
-    <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52"/>
-      <c r="B13" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="45"/>
-      <c r="H13" s="53" t="s">
-        <v>189</v>
-      </c>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
-      <c r="M13" s="54"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="55"/>
-    </row>
-    <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="50"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="57"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="57"/>
-      <c r="N14" s="57"/>
-      <c r="O14" s="58"/>
-    </row>
-    <row r="15" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="48" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="50"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="57"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="57"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="57"/>
-      <c r="N15" s="57"/>
-      <c r="O15" s="58"/>
-    </row>
-    <row r="16" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="H16" s="56"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="58"/>
-    </row>
-    <row r="17" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
-      <c r="B17" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="H17" s="56"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
-      <c r="O17" s="58"/>
-    </row>
-    <row r="18" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="52"/>
-      <c r="B18" s="48" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="50" t="s">
+      <c r="H18" s="55"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="56"/>
+      <c r="M18" s="56"/>
+      <c r="N18" s="56"/>
+      <c r="O18" s="57"/>
+    </row>
+    <row r="19" spans="1:15" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="49"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="56"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="56"/>
+      <c r="O19" s="57"/>
+    </row>
+    <row r="20" spans="1:15" s="24" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
+      <c r="B20" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="55"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="56"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="57"/>
+    </row>
+    <row r="21" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="51"/>
+      <c r="B21" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="55"/>
+      <c r="I21" s="56"/>
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="57"/>
+    </row>
+    <row r="22" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
+      <c r="B22" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="55"/>
+      <c r="I22" s="56"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="56"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="57"/>
+    </row>
+    <row r="23" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="51"/>
+      <c r="B23" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="H18" s="56"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-      <c r="O18" s="58"/>
-    </row>
-    <row r="19" spans="1:15" s="42" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52"/>
-      <c r="B19" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="50"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="58"/>
-    </row>
-    <row r="20" spans="1:15" s="24" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="52"/>
-      <c r="B20" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="56"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="58"/>
-    </row>
-    <row r="21" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="56"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="58"/>
-    </row>
-    <row r="22" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="52"/>
-      <c r="B22" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="H22" s="56"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="57"/>
-      <c r="K22" s="57"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="57"/>
-      <c r="N22" s="57"/>
-      <c r="O22" s="58"/>
-    </row>
-    <row r="23" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="52"/>
-      <c r="B23" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="H23" s="56"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="57"/>
-      <c r="K23" s="57"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="57"/>
-      <c r="N23" s="57"/>
-      <c r="O23" s="58"/>
+      <c r="H23" s="55"/>
+      <c r="I23" s="56"/>
+      <c r="J23" s="56"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="56"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="57"/>
     </row>
     <row r="24" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="51"/>
+      <c r="B24" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="50" t="s">
+      <c r="C24" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="56"/>
-      <c r="I24" s="57"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="57"/>
-      <c r="N24" s="57"/>
-      <c r="O24" s="58"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="56"/>
+      <c r="J24" s="56"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="56"/>
+      <c r="M24" s="56"/>
+      <c r="N24" s="56"/>
+      <c r="O24" s="57"/>
     </row>
     <row r="25" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
-      <c r="B25" s="48" t="s">
+      <c r="A25" s="51"/>
+      <c r="B25" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="60"/>
-      <c r="N25" s="60"/>
-      <c r="O25" s="61"/>
+      <c r="C25" s="49"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="60"/>
     </row>
     <row r="26" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
-      <c r="B26" s="49" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="50"/>
+      <c r="C26" s="49"/>
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
       <c r="J26" s="22"/>
@@ -3542,11 +3780,11 @@
       <c r="O26" s="22"/>
     </row>
     <row r="27" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="52"/>
-      <c r="B27" s="49" t="s">
+      <c r="A27" s="51"/>
+      <c r="B27" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="50"/>
+      <c r="C27" s="49"/>
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
       <c r="J27" s="22"/>
@@ -3557,11 +3795,11 @@
       <c r="O27" s="22"/>
     </row>
     <row r="28" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="52"/>
-      <c r="B28" s="49" t="s">
+      <c r="A28" s="51"/>
+      <c r="B28" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C28" s="50"/>
+      <c r="C28" s="49"/>
       <c r="H28" s="22"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
@@ -3572,12 +3810,12 @@
       <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="52"/>
-      <c r="B29" s="49" t="s">
+      <c r="A29" s="51"/>
+      <c r="B29" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="50" t="s">
-        <v>184</v>
+      <c r="C29" s="49" t="s">
+        <v>183</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
@@ -3589,12 +3827,12 @@
       <c r="O29" s="22"/>
     </row>
     <row r="30" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="52"/>
-      <c r="B30" s="49" t="s">
+      <c r="A30" s="51"/>
+      <c r="B30" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="50" t="s">
-        <v>185</v>
+      <c r="C30" s="49" t="s">
+        <v>184</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -3606,12 +3844,12 @@
       <c r="O30" s="22"/>
     </row>
     <row r="31" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="49" t="s">
+      <c r="A31" s="51"/>
+      <c r="B31" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="50" t="s">
-        <v>185</v>
+      <c r="C31" s="49" t="s">
+        <v>184</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
@@ -3623,12 +3861,12 @@
       <c r="O31" s="22"/>
     </row>
     <row r="32" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="49" t="s">
+      <c r="A32" s="51"/>
+      <c r="B32" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="50" t="s">
-        <v>186</v>
+      <c r="C32" s="49" t="s">
+        <v>185</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
@@ -3640,12 +3878,12 @@
       <c r="O32" s="22"/>
     </row>
     <row r="33" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="52"/>
-      <c r="B33" s="49" t="s">
+      <c r="A33" s="51"/>
+      <c r="B33" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="50" t="s">
-        <v>187</v>
+      <c r="C33" s="49" t="s">
+        <v>186</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -3657,100 +3895,100 @@
       <c r="O33" s="22"/>
     </row>
     <row r="34" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="52"/>
-      <c r="B34" s="49" t="s">
+      <c r="A34" s="51"/>
+      <c r="B34" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="50" t="s">
-        <v>184</v>
+      <c r="C34" s="49" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="49" t="s">
+      <c r="A35" s="51"/>
+      <c r="B35" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="50"/>
+      <c r="C35" s="49"/>
     </row>
     <row r="36" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="52"/>
-      <c r="B36" s="49" t="s">
+      <c r="A36" s="51"/>
+      <c r="B36" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="49" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="49" t="s">
+      <c r="A37" s="51"/>
+      <c r="B37" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="49" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
-      <c r="B38" s="49" t="s">
+      <c r="A38" s="51"/>
+      <c r="B38" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="50" t="s">
+      <c r="C38" s="49" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="52"/>
+      <c r="A39" s="51"/>
       <c r="B39" s="15"/>
       <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="52"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="15"/>
       <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
+      <c r="A41" s="51"/>
       <c r="B41" s="15"/>
       <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="52"/>
+      <c r="A42" s="51"/>
       <c r="B42" s="15"/>
       <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="52"/>
+      <c r="A43" s="51"/>
       <c r="B43" s="15"/>
       <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="52"/>
+      <c r="A44" s="51"/>
       <c r="B44" s="15"/>
       <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="52"/>
+      <c r="A45" s="51"/>
       <c r="B45" s="15"/>
       <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="52"/>
+      <c r="A46" s="51"/>
       <c r="B46" s="20"/>
       <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="52"/>
+      <c r="A47" s="51"/>
       <c r="B47"/>
       <c r="C47"/>
     </row>
     <row r="48" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="52"/>
+      <c r="A48" s="51"/>
       <c r="B48"/>
       <c r="C48"/>
     </row>
     <row r="49" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="52"/>
+      <c r="A49" s="51"/>
       <c r="B49"/>
       <c r="C49"/>
     </row>
@@ -3801,14 +4039,14 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:CO2"/>
+  <dimension ref="A1:CO4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD29"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3817,19 +4055,18 @@
     <col min="2" max="2" width="8.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="4.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="77.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.140625" style="46" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.140625" style="45" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="26.5703125" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="23.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.140625" style="46" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.140625" style="45" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="29.85546875" style="13" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="32.5703125" style="2" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="23" style="27" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23" style="28" customWidth="1"/>
-    <col min="13" max="93" width="9.140625" style="1"/>
+    <col min="12" max="93" width="9.140625" style="1"/>
     <col min="94" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
@@ -3852,10 +4089,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>52</v>
@@ -3863,95 +4100,198 @@
       <c r="K1" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="D2" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>13</v>
+        <v>174</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>229</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>229</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K1 K3:K6">
-    <cfRule type="cellIs" dxfId="121" priority="3311" operator="equal">
+  <conditionalFormatting sqref="K8:K10 K14:K16 K1 K4:K6">
+    <cfRule type="cellIs" dxfId="132" priority="3322" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="3312" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="3323" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K1 K3:K6">
-    <cfRule type="containsText" dxfId="119" priority="3309" operator="containsText" text="pass">
+  <conditionalFormatting sqref="K8:K10 K14:K16 K1 K4:K6">
+    <cfRule type="containsText" dxfId="130" priority="3320" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="3310" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="129" priority="3321" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K3:K6">
-    <cfRule type="cellIs" dxfId="117" priority="3307" operator="equal">
+  <conditionalFormatting sqref="K8:K10 K14:K16 K4:K6">
+    <cfRule type="cellIs" dxfId="128" priority="3318" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="3308" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K3:K6">
-    <cfRule type="containsText" dxfId="115" priority="3306" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K1 K3:L1048576">
-    <cfRule type="containsText" dxfId="114" priority="3303" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="127" priority="3319" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8:K10 K14:K16 K4:K6">
+    <cfRule type="containsText" dxfId="126" priority="3317" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1 K4:K1048576">
+    <cfRule type="containsText" dxfId="125" priority="3314" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="3304" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="124" priority="3315" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="3305" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="123" priority="3316" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K1 K3:L1048576">
-    <cfRule type="cellIs" dxfId="111" priority="3302" operator="equal">
+  <conditionalFormatting sqref="K1 K4:K1048576">
+    <cfRule type="cellIs" dxfId="122" priority="3313" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="110" priority="119" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="121" priority="130" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="120" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="120" priority="131" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="121" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="119" priority="132" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="107" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="129" operator="equal">
+      <formula>"ReWrite Test"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11 K13">
+    <cfRule type="cellIs" dxfId="117" priority="149" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="150" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11 K13">
+    <cfRule type="containsText" dxfId="115" priority="147" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="148" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11 K13">
+    <cfRule type="cellIs" dxfId="113" priority="145" operator="equal">
+      <formula>"Incomplete"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="146" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11 K13">
+    <cfRule type="containsText" dxfId="111" priority="144" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11 K13">
+    <cfRule type="containsText" dxfId="110" priority="141" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="142" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="143" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11 K13">
+    <cfRule type="cellIs" dxfId="107" priority="140" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3984,64 +4324,64 @@
       <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="99" priority="130" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="131" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="132" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="96" priority="129" operator="equal">
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="99" priority="100" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="101" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="97" priority="102" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="cellIs" dxfId="96" priority="99" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="95" priority="127" operator="equal">
+  <conditionalFormatting sqref="K12">
+    <cfRule type="cellIs" dxfId="95" priority="119" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="120" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="93" priority="125" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="126" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="91" priority="123" operator="equal">
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="93" priority="117" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="92" priority="118" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="cellIs" dxfId="91" priority="115" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="124" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="89" priority="122" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
+    <cfRule type="containsText" dxfId="90" priority="116" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="89" priority="114" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="containsText" dxfId="88" priority="111" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="87" priority="112" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="91" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="86" priority="113" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="85" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="110" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4074,322 +4414,322 @@
       <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="77" priority="100" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="101" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="102" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="74" priority="99" operator="equal">
+  <conditionalFormatting sqref="K7">
+    <cfRule type="cellIs" dxfId="77" priority="89" operator="equal">
+      <formula>"Failed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="90" operator="equal">
+      <formula>"Passed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="75" priority="87" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="74" priority="88" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="cellIs" dxfId="73" priority="85" operator="equal">
+      <formula>"Incomplete"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="72" priority="86" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="71" priority="84" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsText" dxfId="70" priority="81" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="82" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="68" priority="83" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K7)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="cellIs" dxfId="67" priority="80" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="73" priority="97" operator="equal">
+  <conditionalFormatting sqref="K19:K24">
+    <cfRule type="cellIs" dxfId="66" priority="74" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="71" priority="95" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="96" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="69" priority="93" operator="equal">
+  <conditionalFormatting sqref="K19:K24">
+    <cfRule type="containsText" dxfId="64" priority="72" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="73" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:K24">
+    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="94" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="67" priority="92" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="66" priority="78" operator="equal">
+    <cfRule type="containsText" dxfId="61" priority="71" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:K24">
+    <cfRule type="containsText" dxfId="60" priority="69" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:K24">
+    <cfRule type="containsText" dxfId="59" priority="66" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="67" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="57" priority="68" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19:K24">
+    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
+      <formula>"ReWrite Test"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="64" priority="76" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="77" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="62" priority="74" operator="equal">
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="53" priority="57" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="58" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="75" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="60" priority="73" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="59" priority="70" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="71" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="72" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="56" priority="69" operator="equal">
+    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="49" priority="54" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="48" priority="51" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="47" priority="52" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="46" priority="53" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="45" priority="50" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K24">
-    <cfRule type="cellIs" dxfId="55" priority="63" operator="equal">
+  <conditionalFormatting sqref="K18">
+    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="45" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K24">
-    <cfRule type="containsText" dxfId="53" priority="61" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="62" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K24">
-    <cfRule type="cellIs" dxfId="51" priority="59" operator="equal">
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="42" priority="42" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="43" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="cellIs" dxfId="40" priority="40" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="60" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K24">
-    <cfRule type="containsText" dxfId="49" priority="58" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K24">
-    <cfRule type="containsText" dxfId="48" priority="55" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="56" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="57" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K24">
-    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+    <cfRule type="containsText" dxfId="39" priority="41" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="38" priority="39" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="containsText" dxfId="37" priority="36" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="35" priority="38" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+  <conditionalFormatting sqref="E26:E1048576">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25:H1048576">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E25 H2:H24">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E25 H2:H24">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="47" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
+  <conditionalFormatting sqref="K2">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="45" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="38" priority="43" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="containsText" dxfId="37" priority="40" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="42" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+  <conditionalFormatting sqref="E2:E25">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H24">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+      <formula>"yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="pass">
+      <formula>NOT(ISERROR(SEARCH("pass",K3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="fail">
+      <formula>NOT(ISERROR(SEARCH("fail",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K18)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K18)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Complete">
+      <formula>NOT(ISERROR(SEARCH("Complete",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Review">
+      <formula>NOT(ISERROR(SEARCH("Review",K3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Rework">
+      <formula>NOT(ISERROR(SEARCH("Rework",K3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Pending">
+      <formula>NOT(ISERROR(SEARCH("Pending",K3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ReWrite Test"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E1048576">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25:H1048576">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25 H2:H24">
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25 H2:H24">
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",E2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="13" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
-      <formula>"Incomplete"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:L2">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:L2">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
-      <formula>"ReWrite Test"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H24">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4415,7 +4755,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4424,7 +4764,7 @@
     <col min="2" max="2" width="34.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="27.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="41"/>
+    <col min="5" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4438,18 +4778,18 @@
         <v>40</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
+      <c r="A2" s="61" t="s">
+        <v>230</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="62" t="s">
         <v>173</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>191</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>59</v>
@@ -4475,7 +4815,7 @@
     <col min="2" max="2" width="34.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="23" style="3" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="27.28515625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="41"/>
+    <col min="5" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4489,18 +4829,18 @@
         <v>40</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>173</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="D2" s="11"/>
     </row>
@@ -4508,11 +4848,11 @@
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>174</v>
+      <c r="B3" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>173</v>
       </c>
       <c r="D3" s="11"/>
     </row>
@@ -4520,11 +4860,11 @@
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>173</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -4532,71 +4872,71 @@
       <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
       <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
       <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
       <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
       <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
       <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="29"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
       <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
       <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="11"/>
       <c r="D13" s="11"/>
     </row>
@@ -4604,7 +4944,7 @@
       <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
     </row>
@@ -4612,7 +4952,7 @@
       <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11"/>
     </row>
@@ -4620,7 +4960,7 @@
       <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
     </row>
@@ -4628,7 +4968,7 @@
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
     </row>
@@ -4636,7 +4976,7 @@
       <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="29"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
     </row>
@@ -4644,7 +4984,7 @@
       <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="29"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
     </row>
@@ -4652,7 +4992,7 @@
       <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="29"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
@@ -4660,7 +5000,7 @@
       <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="29"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
     </row>
@@ -4675,198 +5015,640 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.85546875" style="35" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="41.140625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="16384" width="9.140625" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+    </row>
+    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29"/>
+      <c r="B8" s="34"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="34"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.28515625" style="35" customWidth="1" collapsed="1"/>
+    <col min="3" max="16384" width="9.140625" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="29">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="29">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="29">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <v>16</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>17</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="29">
+        <v>18</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <v>19</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="29">
+        <v>20</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="29">
+        <v>21</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29">
+        <v>22</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29">
+        <v>23</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <v>24</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="29">
+        <v>25</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="29">
+        <v>26</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="29">
+        <v>27</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="29">
+        <v>29</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.140625" style="36" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.28515625" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.140625" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.42578125" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.85546875" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.7109375" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.5703125" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.85546875" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.42578125" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.7109375" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.5703125" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="9.140625" style="34"/>
+    <col min="1" max="1" width="7.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.140625" style="35" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.85546875" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="34.28515625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.140625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.85546875" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.7109375" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.5703125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.85546875" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="24.7109375" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="22.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>110</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="M1" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="P1" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>71</v>
+      <c r="Q1" s="32" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="35"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="6"/>
-      <c r="F2" s="38"/>
-      <c r="H2" s="40"/>
-      <c r="P2" s="38"/>
+      <c r="F2" s="37"/>
+      <c r="H2" s="39"/>
+      <c r="P2" s="37"/>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="35"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="6"/>
-      <c r="F3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="P3" s="38"/>
+      <c r="F3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="P3" s="37"/>
     </row>
     <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="6"/>
-      <c r="P4" s="38"/>
+      <c r="P4" s="37"/>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="6"/>
-      <c r="P5" s="38"/>
+      <c r="P5" s="37"/>
     </row>
     <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="6"/>
-      <c r="P6" s="38"/>
+      <c r="P6" s="37"/>
     </row>
     <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="35"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="6"/>
-      <c r="P7" s="38"/>
+      <c r="P7" s="37"/>
     </row>
     <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="6"/>
-      <c r="P8" s="38"/>
+      <c r="P8" s="37"/>
     </row>
     <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="6"/>
-      <c r="P9" s="38"/>
+      <c r="P9" s="37"/>
     </row>
     <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="6"/>
-      <c r="P10" s="38"/>
+      <c r="P10" s="37"/>
     </row>
     <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="6"/>
-      <c r="P11" s="38"/>
+      <c r="P11" s="37"/>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="6"/>
-      <c r="P12" s="38"/>
+      <c r="P12" s="37"/>
     </row>
     <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="35"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="6"/>
-      <c r="P13" s="38"/>
+      <c r="P13" s="37"/>
     </row>
     <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="6"/>
-      <c r="P14" s="38"/>
+      <c r="P14" s="37"/>
     </row>
     <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="35"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="6"/>
-      <c r="P15" s="38"/>
+      <c r="P15" s="37"/>
     </row>
     <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="6"/>
-      <c r="P16" s="38"/>
+      <c r="P16" s="37"/>
     </row>
     <row r="17" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="6"/>
-      <c r="P17" s="38"/>
+      <c r="P17" s="37"/>
     </row>
     <row r="18" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="6"/>
-      <c r="P18" s="38"/>
+      <c r="P18" s="37"/>
     </row>
     <row r="19" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6"/>
-      <c r="P19" s="38"/>
+      <c r="P19" s="37"/>
     </row>
   </sheetData>
   <dataValidations count="4">
@@ -4901,7 +5683,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
+<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4909,15 +5691,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4925,7 +5707,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -4937,25 +5719,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37263D0A-2349-44FA-8C75-E1703737DEBD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA29ACC8-49E5-48E0-A007-3CFF2AA656E1}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: Role Managment : Edit,Delete,Deactivate and View
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
   <si>
     <t>Execution_Flag</t>
   </si>
@@ -735,9 +735,6 @@
     <t>TestRole</t>
   </si>
   <si>
-    <t>دور إختبار</t>
-  </si>
-  <si>
     <t>1-4</t>
   </si>
   <si>
@@ -762,10 +759,34 @@
     <t>AuthorityName</t>
   </si>
   <si>
-    <t>Scenario_01</t>
-  </si>
-  <si>
-    <t>1,2</t>
+    <t>ValidateEditUserRole</t>
+  </si>
+  <si>
+    <t>ValidateDeactivateUserRole</t>
+  </si>
+  <si>
+    <t>ValidateViewDetailsUserRole</t>
+  </si>
+  <si>
+    <t>ValidateDeleteUserRole</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>دورثاني</t>
+  </si>
+  <si>
+    <t>TestSecondRole</t>
+  </si>
+  <si>
+    <t>Validate Edit,Deactivate, View and Delete  User Role</t>
+  </si>
+  <si>
+    <t>دور اختبار</t>
+  </si>
+  <si>
+    <t>5-9</t>
   </si>
 </sst>
 </file>
@@ -1326,6 +1347,13 @@
     <xf numFmtId="49" fontId="5" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1356,13 +1384,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3441,7 +3462,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
+      <c r="A1" s="53"/>
       <c r="B1" s="16" t="s">
         <v>8</v>
       </c>
@@ -3450,7 +3471,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51"/>
+      <c r="A2" s="54"/>
       <c r="B2" s="14" t="s">
         <v>14</v>
       </c>
@@ -3459,7 +3480,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
@@ -3468,7 +3489,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="14" t="s">
         <v>10</v>
       </c>
@@ -3477,7 +3498,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
@@ -3486,7 +3507,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
@@ -3495,7 +3516,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
@@ -3504,7 +3525,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="14" t="s">
         <v>65</v>
       </c>
@@ -3513,7 +3534,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="14" t="s">
         <v>177</v>
       </c>
@@ -3522,7 +3543,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="51"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="14" t="s">
         <v>179</v>
       </c>
@@ -3531,7 +3552,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="51"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="14" t="s">
         <v>42</v>
       </c>
@@ -3541,7 +3562,7 @@
       <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="51"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="14" t="s">
         <v>180</v>
       </c>
@@ -3551,221 +3572,221 @@
       <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="47" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="44"/>
-      <c r="H13" s="52" t="s">
+      <c r="H13" s="55" t="s">
         <v>188</v>
       </c>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="53"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="54"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="56"/>
+      <c r="M13" s="56"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="57"/>
     </row>
     <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="47" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="49"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="57"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="60"/>
     </row>
     <row r="15" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
+      <c r="A15" s="54"/>
       <c r="B15" s="47" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="49"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="57"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="60"/>
     </row>
     <row r="16" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="47" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="57"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="59"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="60"/>
     </row>
     <row r="17" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="47" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="57"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="59"/>
+      <c r="O17" s="60"/>
     </row>
     <row r="18" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
+      <c r="A18" s="54"/>
       <c r="B18" s="47" t="s">
         <v>34</v>
       </c>
       <c r="C18" s="49" t="s">
         <v>181</v>
       </c>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="57"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="59"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="59"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="60"/>
     </row>
     <row r="19" spans="1:15" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="47" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="49"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="60"/>
     </row>
     <row r="20" spans="1:15" s="24" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="47" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="55"/>
-      <c r="I20" s="56"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="57"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="60"/>
     </row>
     <row r="21" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="47" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="H21" s="55"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="57"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="59"/>
+      <c r="J21" s="59"/>
+      <c r="K21" s="59"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="60"/>
     </row>
     <row r="22" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="47" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="H22" s="55"/>
-      <c r="I22" s="56"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="57"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="60"/>
     </row>
     <row r="23" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="47" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="49" t="s">
         <v>182</v>
       </c>
-      <c r="H23" s="55"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="57"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="60"/>
     </row>
     <row r="24" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="51"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="47" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="55"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="57"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="60"/>
     </row>
     <row r="25" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="47" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="49"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="59"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="59"/>
-      <c r="M25" s="59"/>
-      <c r="N25" s="59"/>
-      <c r="O25" s="60"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="62"/>
+      <c r="N25" s="62"/>
+      <c r="O25" s="63"/>
     </row>
     <row r="26" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="48" t="s">
         <v>35</v>
       </c>
@@ -3780,7 +3801,7 @@
       <c r="O26" s="22"/>
     </row>
     <row r="27" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="48" t="s">
         <v>36</v>
       </c>
@@ -3795,7 +3816,7 @@
       <c r="O27" s="22"/>
     </row>
     <row r="28" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="51"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="48" t="s">
         <v>23</v>
       </c>
@@ -3810,7 +3831,7 @@
       <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="48" t="s">
         <v>37</v>
       </c>
@@ -3827,7 +3848,7 @@
       <c r="O29" s="22"/>
     </row>
     <row r="30" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="48" t="s">
         <v>38</v>
       </c>
@@ -3844,7 +3865,7 @@
       <c r="O30" s="22"/>
     </row>
     <row r="31" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="48" t="s">
         <v>39</v>
       </c>
@@ -3861,7 +3882,7 @@
       <c r="O31" s="22"/>
     </row>
     <row r="32" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="48" t="s">
         <v>27</v>
       </c>
@@ -3878,7 +3899,7 @@
       <c r="O32" s="22"/>
     </row>
     <row r="33" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="51"/>
+      <c r="A33" s="54"/>
       <c r="B33" s="48" t="s">
         <v>24</v>
       </c>
@@ -3895,7 +3916,7 @@
       <c r="O33" s="22"/>
     </row>
     <row r="34" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="51"/>
+      <c r="A34" s="54"/>
       <c r="B34" s="48" t="s">
         <v>25</v>
       </c>
@@ -3904,14 +3925,14 @@
       </c>
     </row>
     <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
+      <c r="A35" s="54"/>
       <c r="B35" s="48" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="49"/>
     </row>
     <row r="36" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
+      <c r="A36" s="54"/>
       <c r="B36" s="48" t="s">
         <v>29</v>
       </c>
@@ -3920,7 +3941,7 @@
       </c>
     </row>
     <row r="37" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="51"/>
+      <c r="A37" s="54"/>
       <c r="B37" s="48" t="s">
         <v>31</v>
       </c>
@@ -3929,7 +3950,7 @@
       </c>
     </row>
     <row r="38" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="51"/>
+      <c r="A38" s="54"/>
       <c r="B38" s="48" t="s">
         <v>30</v>
       </c>
@@ -3938,57 +3959,57 @@
       </c>
     </row>
     <row r="39" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
+      <c r="A39" s="54"/>
       <c r="B39" s="15"/>
       <c r="C39" s="7"/>
     </row>
     <row r="40" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="51"/>
+      <c r="A40" s="54"/>
       <c r="B40" s="15"/>
       <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
+      <c r="A41" s="54"/>
       <c r="B41" s="15"/>
       <c r="C41" s="7"/>
     </row>
     <row r="42" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="51"/>
+      <c r="A42" s="54"/>
       <c r="B42" s="15"/>
       <c r="C42" s="7"/>
     </row>
     <row r="43" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
+      <c r="A43" s="54"/>
       <c r="B43" s="15"/>
       <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="51"/>
+      <c r="A44" s="54"/>
       <c r="B44" s="15"/>
       <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="51"/>
+      <c r="A45" s="54"/>
       <c r="B45" s="15"/>
       <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="51"/>
+      <c r="A46" s="54"/>
       <c r="B46" s="20"/>
       <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="51"/>
+      <c r="A47" s="54"/>
       <c r="B47"/>
       <c r="C47"/>
     </row>
     <row r="48" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="51"/>
+      <c r="A48" s="54"/>
       <c r="B48"/>
       <c r="C48"/>
     </row>
     <row r="49" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="51"/>
+      <c r="A49" s="54"/>
       <c r="B49"/>
       <c r="C49"/>
     </row>
@@ -4039,14 +4060,14 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:CO4"/>
+  <dimension ref="A1:CO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4109,13 +4130,13 @@
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>174</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>191</v>
@@ -4138,19 +4159,19 @@
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>229</v>
+        <v>13</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>118</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>56</v>
@@ -4166,20 +4187,20 @@
       <c r="B4" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="D4" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E4" s="45" t="s">
         <v>13</v>
       </c>
+      <c r="F4" s="13" t="s">
+        <v>118</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="H4" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>56</v>
@@ -4188,8 +4209,95 @@
         <v>71</v>
       </c>
     </row>
+    <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K1 K4:K6">
+  <conditionalFormatting sqref="K14:K16 K1 K4:K10">
     <cfRule type="cellIs" dxfId="132" priority="3322" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
@@ -4197,7 +4305,7 @@
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K1 K4:K6">
+  <conditionalFormatting sqref="K14:K16 K1 K4:K10">
     <cfRule type="containsText" dxfId="130" priority="3320" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K1)))</formula>
     </cfRule>
@@ -4205,7 +4313,7 @@
       <formula>NOT(ISERROR(SEARCH("fail",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K4:K6">
+  <conditionalFormatting sqref="K14:K16 K4:K10">
     <cfRule type="cellIs" dxfId="128" priority="3318" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
@@ -4213,7 +4321,7 @@
       <formula>NOT(ISERROR(SEARCH("Complete",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10 K14:K16 K4:K6">
+  <conditionalFormatting sqref="K14:K16 K4:K10">
     <cfRule type="containsText" dxfId="126" priority="3317" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K4)))</formula>
     </cfRule>
@@ -4414,51 +4522,6 @@
       <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="77" priority="89" operator="equal">
-      <formula>"Failed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="90" operator="equal">
-      <formula>"Passed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="75" priority="87" operator="containsText" text="pass">
-      <formula>NOT(ISERROR(SEARCH("pass",K7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="88" operator="containsText" text="fail">
-      <formula>NOT(ISERROR(SEARCH("fail",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="73" priority="85" operator="equal">
-      <formula>"Incomplete"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="86" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="71" priority="84" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="containsText" dxfId="70" priority="81" operator="containsText" text="Review">
-      <formula>NOT(ISERROR(SEARCH("Review",K7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="82" operator="containsText" text="Rework">
-      <formula>NOT(ISERROR(SEARCH("Rework",K7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="83" operator="containsText" text="Pending">
-      <formula>NOT(ISERROR(SEARCH("Pending",K7)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="67" priority="80" operator="equal">
-      <formula>"ReWrite Test"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K19:K24">
     <cfRule type="cellIs" dxfId="66" priority="74" operator="equal">
       <formula>"Failed"</formula>
@@ -4733,7 +4796,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576 H2:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576 E2:E1048576">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4782,13 +4845,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
-        <v>230</v>
+      <c r="A2" s="50" t="s">
+        <v>229</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="51" t="s">
         <v>173</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -5017,8 +5080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5044,7 +5107,7 @@
         <v>41</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>222</v>
@@ -5067,25 +5130,40 @@
         <v>221</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E2" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>240</v>
+      </c>
+      <c r="G2" s="35" t="s">
         <v>226</v>
       </c>
-      <c r="F2" s="39" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="29">
+        <v>2</v>
+      </c>
+      <c r="B3" s="34">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="F3" s="39" t="s">
         <v>225</v>
       </c>
-      <c r="G2" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
+      <c r="G3" s="35" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
@@ -5206,7 +5284,7 @@
   <cols>
     <col min="1" max="1" width="7.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="42.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="63"/>
+    <col min="3" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5214,7 +5292,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5737,7 +5815,7 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FA29ACC8-49E5-48E0-A007-3CFF2AA656E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{233E76D2-B652-4F25-80CE-D02077DC80FD}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: Role Managment : Edit,Delete,Deactivate /Activate and View
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -762,9 +762,6 @@
     <t>ValidateEditUserRole</t>
   </si>
   <si>
-    <t>ValidateDeactivateUserRole</t>
-  </si>
-  <si>
     <t>ValidateViewDetailsUserRole</t>
   </si>
   <si>
@@ -787,6 +784,9 @@
   </si>
   <si>
     <t>5-9</t>
+  </si>
+  <si>
+    <t>ValidateChangeStatusUserRole</t>
   </si>
 </sst>
 </file>
@@ -4062,12 +4062,12 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CO7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4200,7 +4200,7 @@
         <v>118</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>56</v>
@@ -4220,7 +4220,7 @@
         <v>230</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>13</v>
@@ -4229,7 +4229,7 @@
         <v>118</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>56</v>
@@ -4249,7 +4249,7 @@
         <v>230</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" s="45" t="s">
         <v>13</v>
@@ -4258,7 +4258,7 @@
         <v>118</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>56</v>
@@ -4278,7 +4278,7 @@
         <v>230</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E7" s="45" t="s">
         <v>13</v>
@@ -4287,7 +4287,7 @@
         <v>118</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>56</v>
@@ -5080,7 +5080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -5133,10 +5133,10 @@
         <v>232</v>
       </c>
       <c r="E2" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="F2" s="39" t="s">
         <v>239</v>
-      </c>
-      <c r="F2" s="39" t="s">
-        <v>240</v>
       </c>
       <c r="G2" s="35" t="s">
         <v>226</v>
@@ -5150,19 +5150,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>232</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F3" s="39" t="s">
         <v>225</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5815,7 +5815,7 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{233E76D2-B652-4F25-80CE-D02077DC80FD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B4D2F60-1CDD-48ED-BA6A-8E79CFD035EB}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: User Management : Identify Elements
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -732,9 +732,6 @@
     <t>RoleAuthorities</t>
   </si>
   <si>
-    <t>TestRole</t>
-  </si>
-  <si>
     <t>1-4</t>
   </si>
   <si>
@@ -787,6 +784,9 @@
   </si>
   <si>
     <t>ValidateChangeStatusUserRole</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -1391,7 +1391,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="133">
+  <dxfs count="122">
     <dxf>
       <fill>
         <patternFill>
@@ -1716,109 +1716,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4062,7 +3959,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CO7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
@@ -4130,13 +4027,13 @@
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>174</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>191</v>
@@ -4159,10 +4056,10 @@
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>13</v>
@@ -4171,7 +4068,7 @@
         <v>118</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>56</v>
@@ -4188,10 +4085,10 @@
         <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E4" s="45" t="s">
         <v>13</v>
@@ -4200,7 +4097,7 @@
         <v>118</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>56</v>
@@ -4217,10 +4114,10 @@
         <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E5" s="45" t="s">
         <v>13</v>
@@ -4229,7 +4126,7 @@
         <v>118</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>56</v>
@@ -4246,10 +4143,10 @@
         <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E6" s="45" t="s">
         <v>13</v>
@@ -4258,7 +4155,7 @@
         <v>118</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>56</v>
@@ -4275,10 +4172,10 @@
         <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E7" s="45" t="s">
         <v>13</v>
@@ -4287,7 +4184,7 @@
         <v>118</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>56</v>
@@ -4298,227 +4195,227 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K14:K16 K1 K4:K10">
-    <cfRule type="cellIs" dxfId="132" priority="3322" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="3322" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="3323" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="3323" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:K16 K1 K4:K10">
-    <cfRule type="containsText" dxfId="130" priority="3320" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="119" priority="3320" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="129" priority="3321" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="118" priority="3321" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:K16 K4:K10">
-    <cfRule type="cellIs" dxfId="128" priority="3318" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="3318" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="3319" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="116" priority="3319" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:K16 K4:K10">
-    <cfRule type="containsText" dxfId="126" priority="3317" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="115" priority="3317" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1 K4:K1048576">
-    <cfRule type="containsText" dxfId="125" priority="3314" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="114" priority="3314" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="3315" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="113" priority="3315" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="3316" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="112" priority="3316" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1 K4:K1048576">
-    <cfRule type="cellIs" dxfId="122" priority="3313" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="3313" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="121" priority="130" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="110" priority="130" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="131" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="109" priority="131" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="132" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="108" priority="132" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="118" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="129" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="117" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="149" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="150" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="115" priority="147" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="104" priority="147" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="148" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="103" priority="148" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="113" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="145" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="146" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="101" priority="146" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="111" priority="144" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="100" priority="144" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="110" priority="141" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="99" priority="141" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="142" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="98" priority="142" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="143" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="97" priority="143" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="107" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="140" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="106" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="138" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="139" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="104" priority="136" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="93" priority="136" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="137" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="92" priority="137" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="cellIs" dxfId="102" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="134" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="135" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="90" priority="135" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11 K13">
-    <cfRule type="containsText" dxfId="100" priority="133" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="89" priority="133" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="99" priority="100" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="88" priority="100" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="101" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="87" priority="101" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="102" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="86" priority="102" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="96" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="99" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="95" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="119" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="120" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="93" priority="117" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="82" priority="117" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="118" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="81" priority="118" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="91" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="115" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="116" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="79" priority="116" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="89" priority="114" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="78" priority="114" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="88" priority="111" operator="containsText" text="Review">
+    <cfRule type="containsText" dxfId="77" priority="111" operator="containsText" text="Review">
       <formula>NOT(ISERROR(SEARCH("Review",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="112" operator="containsText" text="Rework">
+    <cfRule type="containsText" dxfId="76" priority="112" operator="containsText" text="Rework">
       <formula>NOT(ISERROR(SEARCH("Rework",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="113" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="75" priority="113" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="85" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="110" operator="equal">
       <formula>"ReWrite Test"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="84" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="108" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="109" operator="equal">
       <formula>"Passed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="82" priority="106" operator="containsText" text="pass">
+    <cfRule type="containsText" dxfId="71" priority="106" operator="containsText" text="pass">
       <formula>NOT(ISERROR(SEARCH("pass",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="107" operator="containsText" text="fail">
+    <cfRule type="containsText" dxfId="70" priority="107" operator="containsText" text="fail">
       <formula>NOT(ISERROR(SEARCH("fail",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="80" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="104" operator="equal">
       <formula>"Incomplete"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="105" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="68" priority="105" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="containsText" dxfId="78" priority="103" operator="containsText" text="Pending">
+    <cfRule type="containsText" dxfId="67" priority="103" operator="containsText" text="Pending">
       <formula>NOT(ISERROR(SEARCH("Pending",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4846,7 +4743,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>172</v>
@@ -5080,8 +4977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5107,7 +5004,7 @@
         <v>41</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E1" s="32" t="s">
         <v>222</v>
@@ -5130,16 +5027,16 @@
         <v>221</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>232</v>
+        <v>243</v>
       </c>
       <c r="E2" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="F2" s="39" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="39" t="s">
-        <v>239</v>
-      </c>
       <c r="G2" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5150,19 +5047,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="E3" s="37" t="s">
+      <c r="F3" s="39" t="s">
+        <v>238</v>
+      </c>
+      <c r="G3" s="35" t="s">
         <v>241</v>
-      </c>
-      <c r="F3" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5292,7 +5189,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5761,7 +5658,7 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5769,15 +5666,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
+<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5785,7 +5682,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -5797,25 +5694,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6B4D2F60-1CDD-48ED-BA6A-8E79CFD035EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B44FA8A-9D33-4739-B2FE-E501B5250078}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: User Management : Validate Add New USer
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="255">
   <si>
     <t>Execution_Flag</t>
   </si>
@@ -237,15 +237,9 @@
     <t>true</t>
   </si>
   <si>
-    <t>InspectionCenter</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
-    <t>UserSpecialization</t>
-  </si>
-  <si>
     <t>Abdelghany</t>
   </si>
   <si>
@@ -354,15 +348,9 @@
     <t>مفتش طوارئ</t>
   </si>
   <si>
-    <t>UserIdType</t>
-  </si>
-  <si>
     <t>UserIdNumber</t>
   </si>
   <si>
-    <t>UserFullName</t>
-  </si>
-  <si>
     <t>UserGender</t>
   </si>
   <si>
@@ -375,18 +363,6 @@
     <t>UserStatus</t>
   </si>
   <si>
-    <t>UserJobTitle</t>
-  </si>
-  <si>
-    <t>UserRoleLevel</t>
-  </si>
-  <si>
-    <t>UserMobileNumber</t>
-  </si>
-  <si>
-    <t>DailyInspectionCapacity</t>
-  </si>
-  <si>
     <t>UserRoles</t>
   </si>
   <si>
@@ -427,9 +403,6 @@
   </si>
   <si>
     <t>مراقب</t>
-  </si>
-  <si>
-    <t>UserRole</t>
   </si>
   <si>
     <t>رخصة الاعلام</t>
@@ -787,6 +760,66 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Validate Add new User</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>FatherName</t>
+  </si>
+  <si>
+    <t>GrandFatherName</t>
+  </si>
+  <si>
+    <t>FamilyName</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>MainRole</t>
+  </si>
+  <si>
+    <t>AdditionalRole</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>Abdelaziz</t>
+  </si>
+  <si>
+    <t>Elsayed</t>
+  </si>
+  <si>
+    <t>0551367731</t>
+  </si>
+  <si>
+    <t>aelsayed@elm.sa</t>
+  </si>
+  <si>
+    <t>02/11/1985</t>
+  </si>
+  <si>
+    <t>موظف التسجيل</t>
+  </si>
+  <si>
+    <t>مشرف مركز الخدمة</t>
+  </si>
+  <si>
+    <t>UserManagement</t>
+  </si>
+  <si>
+    <t>ValidateAddUser</t>
+  </si>
+  <si>
+    <t>1010101011</t>
   </si>
 </sst>
 </file>
@@ -1213,7 +1246,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1384,6 +1417,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3002,25 +3038,25 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H1" s="38" t="s">
         <v>60</v>
@@ -3029,310 +3065,310 @@
         <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="M1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="N1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H2" s="38" t="s">
         <v>62</v>
       </c>
       <c r="I2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="J2" t="s">
+        <v>139</v>
+      </c>
+      <c r="M2" t="s">
         <v>148</v>
       </c>
-      <c r="M2" t="s">
-        <v>157</v>
-      </c>
       <c r="N2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="I3" t="s">
         <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="K3" s="42" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="M3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="N3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="I4" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="J4" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="K4" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="M4" t="s">
         <v>149</v>
       </c>
-      <c r="L4" s="42" t="s">
-        <v>170</v>
-      </c>
-      <c r="M4" t="s">
-        <v>158</v>
-      </c>
       <c r="N4" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
         <v>64</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I5" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="J5" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="M5" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="N5" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="N6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G7" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="I7" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="J7" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I8" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="J8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="J9" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -3373,7 +3409,7 @@
         <v>14</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3391,7 +3427,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3400,7 +3436,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3409,7 +3445,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3427,22 +3463,22 @@
         <v>65</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
       <c r="B9" s="14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54"/>
       <c r="B10" s="14" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>55</v>
@@ -3454,17 +3490,17 @@
         <v>42</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="54"/>
       <c r="B12" s="14" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="D12" s="44"/>
     </row>
@@ -3476,7 +3512,7 @@
       <c r="C13" s="49"/>
       <c r="D13" s="44"/>
       <c r="H13" s="55" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
@@ -3556,7 +3592,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="H18" s="58"/>
       <c r="I18" s="59"/>
@@ -3639,7 +3675,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="H23" s="58"/>
       <c r="I23" s="59"/>
@@ -3733,7 +3769,7 @@
         <v>37</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
@@ -3750,7 +3786,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -3767,7 +3803,7 @@
         <v>39</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
@@ -3784,7 +3820,7 @@
         <v>27</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
@@ -3801,7 +3837,7 @@
         <v>24</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -3818,7 +3854,7 @@
         <v>25</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3957,14 +3993,14 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:CO7"/>
+  <dimension ref="A1:CO8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4007,10 +4043,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="25" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>52</v>
@@ -4027,25 +4063,25 @@
         <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4056,25 +4092,25 @@
         <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4085,25 +4121,25 @@
         <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E4" s="45" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4114,25 +4150,25 @@
         <v>54</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4143,25 +4179,25 @@
         <v>54</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K6" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4172,25 +4208,54 @@
         <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>13</v>
+        <v>218</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>56</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>218</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4570,7 +4635,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25 H2:H24">
+  <conditionalFormatting sqref="H2:H24 E2:E25">
     <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
     </cfRule>
@@ -4578,7 +4643,7 @@
       <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E25 H2:H24">
+  <conditionalFormatting sqref="H2:H24 E2:E25">
     <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",E2)))</formula>
     </cfRule>
@@ -4738,18 +4803,18 @@
         <v>40</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>59</v>
@@ -4789,7 +4854,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4797,10 +4862,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D2" s="11"/>
     </row>
@@ -4809,10 +4874,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D3" s="11"/>
     </row>
@@ -4821,10 +4886,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -4977,7 +5042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -5004,16 +5069,16 @@
         <v>41</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5024,19 +5089,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5047,19 +5112,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="E3" s="37" t="s">
-        <v>240</v>
-      </c>
       <c r="F3" s="39" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5189,7 +5254,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5197,7 +5262,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5205,7 +5270,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5213,7 +5278,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5221,7 +5286,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5229,7 +5294,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5237,7 +5302,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5245,7 +5310,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5253,7 +5318,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5261,7 +5326,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5269,7 +5334,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5277,7 +5342,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5285,7 +5350,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5293,7 +5358,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5301,7 +5366,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5309,7 +5374,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5317,7 +5382,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5325,7 +5390,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5333,7 +5398,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5341,7 +5406,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5349,7 +5414,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5357,7 +5422,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5365,7 +5430,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5373,7 +5438,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5381,7 +5446,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5389,7 +5454,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5397,7 +5462,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5405,7 +5470,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5413,7 +5478,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5421,7 +5486,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -5432,35 +5497,32 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="10.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.140625" style="35" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.85546875" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.28515625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="34.28515625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.140625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.85546875" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.7109375" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="9.5703125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.85546875" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="24.7109375" style="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="22.5703125" style="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="9.140625" style="33"/>
+    <col min="3" max="3" width="24.140625" style="35" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14.5703125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5703125" style="35" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14.5703125" style="35" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.85546875" style="35" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="15.85546875" style="35" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.42578125" style="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.42578125" style="35" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="17.7109375" style="35" customWidth="1" collapsed="1"/>
+    <col min="16" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>6</v>
       </c>
@@ -5471,194 +5533,199 @@
         <v>41</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="32" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="L1" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="M1" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="M1" s="32" t="s">
-        <v>132</v>
-      </c>
       <c r="N1" s="32" t="s">
-        <v>68</v>
+        <v>241</v>
       </c>
       <c r="O1" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="P1" s="32" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q1" s="32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="6"/>
-      <c r="F2" s="37"/>
-      <c r="H2" s="39"/>
-      <c r="P2" s="37"/>
-    </row>
-    <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>1</v>
+      </c>
+      <c r="B2" s="34">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="K2" s="64" t="s">
+        <v>248</v>
+      </c>
+      <c r="L2" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="M2" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="O2" s="35" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29"/>
       <c r="B3" s="34"/>
       <c r="C3" s="6"/>
+      <c r="E3" s="37"/>
       <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
       <c r="H3" s="37"/>
-      <c r="P3" s="37"/>
-    </row>
-    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="37"/>
+      <c r="K3" s="37"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29"/>
       <c r="B4" s="34"/>
       <c r="C4" s="6"/>
-      <c r="P4" s="37"/>
-    </row>
-    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29"/>
       <c r="B5" s="34"/>
       <c r="C5" s="6"/>
-      <c r="P5" s="37"/>
-    </row>
-    <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29"/>
       <c r="B6" s="34"/>
       <c r="C6" s="6"/>
-      <c r="P6" s="37"/>
-    </row>
-    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29"/>
       <c r="B7" s="34"/>
       <c r="C7" s="6"/>
-      <c r="P7" s="37"/>
-    </row>
-    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29"/>
       <c r="B8" s="34"/>
       <c r="C8" s="6"/>
-      <c r="P8" s="37"/>
-    </row>
-    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29"/>
       <c r="B9" s="34"/>
       <c r="C9" s="6"/>
-      <c r="P9" s="37"/>
-    </row>
-    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="34"/>
       <c r="C10" s="6"/>
-      <c r="P10" s="37"/>
-    </row>
-    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
       <c r="B11" s="34"/>
       <c r="C11" s="6"/>
-      <c r="P11" s="37"/>
-    </row>
-    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="34"/>
       <c r="C12" s="6"/>
-      <c r="P12" s="37"/>
-    </row>
-    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29"/>
       <c r="B13" s="34"/>
       <c r="C13" s="6"/>
-      <c r="P13" s="37"/>
-    </row>
-    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29"/>
       <c r="B14" s="34"/>
       <c r="C14" s="6"/>
-      <c r="P14" s="37"/>
-    </row>
-    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="34"/>
       <c r="C15" s="6"/>
-      <c r="P15" s="37"/>
-    </row>
-    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29"/>
       <c r="B16" s="34"/>
       <c r="C16" s="6"/>
-      <c r="P16" s="37"/>
-    </row>
-    <row r="17" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="34"/>
       <c r="C17" s="6"/>
-      <c r="P17" s="37"/>
-    </row>
-    <row r="18" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29"/>
       <c r="B18" s="34"/>
       <c r="C18" s="6"/>
-      <c r="P18" s="37"/>
-    </row>
-    <row r="19" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29"/>
       <c r="B19" s="34"/>
       <c r="C19" s="6"/>
-      <c r="P19" s="37"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"هوية وطنية,هوية مقيم"</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
+      <formula1>"male,female"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576">
-      <formula1>"ذكر,أنثى"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576">
-      <formula1>"فعال,غير فعال"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
-      <formula1>"إدارة النظام,مركز التفتيش,إدارة مراكز التفتيش"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576">
+      <formula1>"active,inactive"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>LookUp!$G$2:$G$16</xm:f>
-          </x14:formula1>
-          <xm:sqref>M2:M1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
+<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5666,15 +5733,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5682,7 +5749,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -5694,25 +5761,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B44FA8A-9D33-4739-B2FE-E501B5250078}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBF02E86-9097-4AF2-A392-51D51EB51EE7}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: Role Management : support Arabic & English system layout.
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="280">
   <si>
     <t>Execution_Flag</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>RunType</t>
-  </si>
-  <si>
-    <t>ENG</t>
   </si>
   <si>
     <t>YES</t>
@@ -672,9 +669,6 @@
     <t>Add Printing Request</t>
   </si>
   <si>
-    <t>Manage Requests</t>
-  </si>
-  <si>
     <t>View Request Details</t>
   </si>
   <si>
@@ -687,9 +681,6 @@
     <t>Update My Profile</t>
   </si>
   <si>
-    <t>Register Hamlah</t>
-  </si>
-  <si>
     <t>Enquiry Hamlah Registration</t>
   </si>
   <si>
@@ -741,18 +732,9 @@
     <t>2</t>
   </si>
   <si>
-    <t>دورثاني</t>
-  </si>
-  <si>
-    <t>TestSecondRole</t>
-  </si>
-  <si>
     <t>Validate Edit,Deactivate, View and Delete  User Role</t>
   </si>
   <si>
-    <t>دور اختبار</t>
-  </si>
-  <si>
     <t>5-9</t>
   </si>
   <si>
@@ -820,6 +802,99 @@
   </si>
   <si>
     <t>1010101011</t>
+  </si>
+  <si>
+    <t>ARB</t>
+  </si>
+  <si>
+    <t>AuthorityNameArb</t>
+  </si>
+  <si>
+    <t>لوحة المعلومات</t>
+  </si>
+  <si>
+    <t>إضافة مستخدم</t>
+  </si>
+  <si>
+    <t>تعديل مستخدم</t>
+  </si>
+  <si>
+    <t>تغيير حالة مستخدم</t>
+  </si>
+  <si>
+    <t>إعادة تعيين كلمة المرور</t>
+  </si>
+  <si>
+    <t>حذف مستخدم</t>
+  </si>
+  <si>
+    <t>إضافة دور</t>
+  </si>
+  <si>
+    <t>تعديل دور</t>
+  </si>
+  <si>
+    <t>حذف دور</t>
+  </si>
+  <si>
+    <t>تغيير حالة دور</t>
+  </si>
+  <si>
+    <t>إعادة تعيين كلمة مرور المستخدم</t>
+  </si>
+  <si>
+    <t>عرض معلومات ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>تعديل معلومات ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>تفعيل بطاقة تعريف ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>إلغاء بطاقة تعريف ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>إيقاف بطاقة تعريف ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>إعادة إصدار بطاقة تعريف ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>إضافة رقم تعريف ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>إنشاء معلومات ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>موافقة إنشاء معلومات ضيف الرحمن</t>
+  </si>
+  <si>
+    <t>عرض تفاصيل طلب الطباعة</t>
+  </si>
+  <si>
+    <t>إضافة طلب طباعة</t>
+  </si>
+  <si>
+    <t>عرض تفاصيل الطلب</t>
+  </si>
+  <si>
+    <t>إنشاء طلب جديد</t>
+  </si>
+  <si>
+    <t>عرض الملف الشخصي</t>
+  </si>
+  <si>
+    <t>تعديل الملف الشخصي</t>
+  </si>
+  <si>
+    <t>استعلام طلب تسجيل حملة</t>
+  </si>
+  <si>
+    <t>TestteestRolessdd</t>
+  </si>
+  <si>
+    <t>دوووور</t>
   </si>
 </sst>
 </file>
@@ -3038,337 +3113,337 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H1" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" t="s">
-        <v>61</v>
-      </c>
       <c r="J1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M1" t="s">
+        <v>149</v>
+      </c>
+      <c r="N1" t="s">
         <v>150</v>
-      </c>
-      <c r="N1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K3" s="42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L3" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="M3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H4" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L4" s="42" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L5" s="42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="M5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L6" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K9" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3383,7 +3458,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3406,10 +3481,10 @@
     <row r="2" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54"/>
       <c r="B2" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3418,7 +3493,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3427,7 +3502,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3436,7 +3511,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3445,7 +3520,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3454,65 +3529,65 @@
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>12</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="54"/>
       <c r="B8" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54"/>
       <c r="B9" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54"/>
       <c r="B10" s="14" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="54"/>
       <c r="B11" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D11" s="44"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="54"/>
       <c r="B12" s="14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D12" s="44"/>
     </row>
     <row r="13" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="54"/>
       <c r="B13" s="47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="49"/>
       <c r="D13" s="44"/>
       <c r="H13" s="55" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
@@ -3525,7 +3600,7 @@
     <row r="14" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="54"/>
       <c r="B14" s="47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="49"/>
       <c r="H14" s="58"/>
@@ -3540,7 +3615,7 @@
     <row r="15" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="54"/>
       <c r="B15" s="47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="49"/>
       <c r="H15" s="58"/>
@@ -3555,10 +3630,10 @@
     <row r="16" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54"/>
       <c r="B16" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="49" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>45</v>
       </c>
       <c r="H16" s="58"/>
       <c r="I16" s="59"/>
@@ -3572,10 +3647,10 @@
     <row r="17" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="54"/>
       <c r="B17" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="49" t="s">
         <v>46</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>47</v>
       </c>
       <c r="H17" s="58"/>
       <c r="I17" s="59"/>
@@ -3589,10 +3664,10 @@
     <row r="18" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="54"/>
       <c r="B18" s="47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H18" s="58"/>
       <c r="I18" s="59"/>
@@ -3606,7 +3681,7 @@
     <row r="19" spans="1:15" s="41" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="54"/>
       <c r="B19" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="49"/>
       <c r="H19" s="58"/>
@@ -3621,10 +3696,10 @@
     <row r="20" spans="1:15" s="24" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="54"/>
       <c r="B20" s="47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H20" s="58"/>
       <c r="I20" s="59"/>
@@ -3638,10 +3713,10 @@
     <row r="21" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="54"/>
       <c r="B21" s="47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21" s="58"/>
       <c r="I21" s="59"/>
@@ -3655,10 +3730,10 @@
     <row r="22" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="54"/>
       <c r="B22" s="47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C22" s="49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H22" s="58"/>
       <c r="I22" s="59"/>
@@ -3672,10 +3747,10 @@
     <row r="23" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="54"/>
       <c r="B23" s="47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H23" s="58"/>
       <c r="I23" s="59"/>
@@ -3689,10 +3764,10 @@
     <row r="24" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="54"/>
       <c r="B24" s="47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C24" s="49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H24" s="58"/>
       <c r="I24" s="59"/>
@@ -3706,7 +3781,7 @@
     <row r="25" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="54"/>
       <c r="B25" s="47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" s="49"/>
       <c r="H25" s="61"/>
@@ -3721,7 +3796,7 @@
     <row r="26" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="54"/>
       <c r="B26" s="48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="49"/>
       <c r="H26" s="22"/>
@@ -3736,7 +3811,7 @@
     <row r="27" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="54"/>
       <c r="B27" s="48" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="49"/>
       <c r="H27" s="22"/>
@@ -3751,7 +3826,7 @@
     <row r="28" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="54"/>
       <c r="B28" s="48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" s="49"/>
       <c r="H28" s="22"/>
@@ -3766,10 +3841,10 @@
     <row r="29" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="54"/>
       <c r="B29" s="48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
@@ -3783,10 +3858,10 @@
     <row r="30" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="54"/>
       <c r="B30" s="48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -3800,10 +3875,10 @@
     <row r="31" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="54"/>
       <c r="B31" s="48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
@@ -3817,10 +3892,10 @@
     <row r="32" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="54"/>
       <c r="B32" s="48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
@@ -3834,10 +3909,10 @@
     <row r="33" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="54"/>
       <c r="B33" s="48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -3851,44 +3926,44 @@
     <row r="34" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="54"/>
       <c r="B34" s="48" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="54"/>
       <c r="B35" s="48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="49"/>
     </row>
     <row r="36" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="54"/>
       <c r="B36" s="48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="54"/>
       <c r="B37" s="48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="54"/>
       <c r="B38" s="48" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3995,12 +4070,12 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CO8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4025,10 +4100,10 @@
         <v>6</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -4043,16 +4118,16 @@
         <v>1</v>
       </c>
       <c r="H1" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>135</v>
-      </c>
       <c r="J1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="26" t="s">
         <v>52</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4060,28 +4135,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E2" s="45" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K2" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4089,28 +4164,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E3" s="45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K3" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4118,28 +4193,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E4" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="J4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K4" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4147,28 +4222,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4176,28 +4251,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K6" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4205,28 +4280,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K7" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -4234,28 +4309,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="E8" s="45" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K8" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -4797,27 +4872,27 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="50" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="51" t="s">
         <v>163</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>164</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -4848,13 +4923,13 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4862,10 +4937,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="28" t="s">
         <v>163</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>164</v>
       </c>
       <c r="D2" s="11"/>
     </row>
@@ -4874,10 +4949,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D3" s="11"/>
     </row>
@@ -4886,10 +4961,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>163</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>164</v>
       </c>
       <c r="D4" s="11"/>
     </row>
@@ -5042,8 +5117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5063,22 +5138,22 @@
         <v>6</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G1" s="32" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5089,19 +5164,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>228</v>
+        <v>279</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>229</v>
+        <v>278</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5112,19 +5187,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>231</v>
+        <v>279</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>229</v>
+        <v>278</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5236,257 +5311,327 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="30" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="42.28515625" style="35" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="52"/>
+    <col min="2" max="3" width="42.28515625" style="35" customWidth="1" collapsed="1"/>
+    <col min="4" max="8" width="9.140625" style="52"/>
+    <col min="9" max="9" width="29.42578125" style="52" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="52"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29">
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29">
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29">
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29">
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29">
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29">
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29">
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="35" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="35" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29">
         <v>16</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>197</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29">
         <v>17</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>18</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+      <c r="C19" s="35" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29">
         <v>19</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29">
         <v>20</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29">
         <v>21</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29">
         <v>22</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29">
         <v>23</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29">
         <v>24</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29">
         <v>25</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29">
         <v>26</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29">
         <v>27</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="35" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29">
-        <v>29</v>
-      </c>
-      <c r="B30" s="35" t="s">
-        <v>211</v>
+        <v>208</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -5527,46 +5672,46 @@
         <v>6</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D1" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="I1" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="J1" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="K1" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="N1" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="O1" s="32" t="s">
         <v>236</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>237</v>
-      </c>
-      <c r="G1" s="32" t="s">
-        <v>238</v>
-      </c>
-      <c r="H1" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="I1" s="32" t="s">
-        <v>240</v>
-      </c>
-      <c r="J1" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="L1" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="M1" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="N1" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="O1" s="32" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5577,43 +5722,43 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F2" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>237</v>
+      </c>
+      <c r="K2" s="64" t="s">
+        <v>242</v>
+      </c>
+      <c r="L2" s="35" t="s">
+        <v>243</v>
+      </c>
+      <c r="M2" s="35" t="s">
+        <v>238</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>244</v>
+      </c>
+      <c r="O2" s="35" t="s">
         <v>245</v>
-      </c>
-      <c r="G2" s="37" t="s">
-        <v>245</v>
-      </c>
-      <c r="H2" s="37" t="s">
-        <v>246</v>
-      </c>
-      <c r="I2" s="37" t="s">
-        <v>247</v>
-      </c>
-      <c r="J2" s="35" t="s">
-        <v>243</v>
-      </c>
-      <c r="K2" s="64" t="s">
-        <v>248</v>
-      </c>
-      <c r="L2" s="35" t="s">
-        <v>249</v>
-      </c>
-      <c r="M2" s="35" t="s">
-        <v>244</v>
-      </c>
-      <c r="N2" s="35" t="s">
-        <v>250</v>
-      </c>
-      <c r="O2" s="35" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -5779,7 +5924,7 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBF02E86-9097-4AF2-A392-51D51EB51EE7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCF376D9-2C5B-4B6F-B274-BB365B1D3937}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: Role Management : support Arabic & English View Role.
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -5118,7 +5118,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5924,7 +5924,7 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCF376D9-2C5B-4B6F-B274-BB365B1D3937}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8696592F-603A-4548-A53B-743BDEA7604D}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: UserManagement : Select role by arabic/english name.
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="313">
   <si>
     <t>Execution_Flag</t>
   </si>
@@ -901,6 +901,99 @@
   </si>
   <si>
     <t>ValidateResetUserPassword</t>
+  </si>
+  <si>
+    <t>1010101013</t>
+  </si>
+  <si>
+    <t>0551367733</t>
+  </si>
+  <si>
+    <t>02/11/1987</t>
+  </si>
+  <si>
+    <t>Validate Add Printing User</t>
+  </si>
+  <si>
+    <t>MainRoleArb</t>
+  </si>
+  <si>
+    <t>AdditionalRoleArb</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>RoleNameArb</t>
+  </si>
+  <si>
+    <t>System Admin</t>
+  </si>
+  <si>
+    <t>System User</t>
+  </si>
+  <si>
+    <t>Enrollment Officer Supervisor</t>
+  </si>
+  <si>
+    <t>Enrollment Officer</t>
+  </si>
+  <si>
+    <t>Service Center Agent Supervisor</t>
+  </si>
+  <si>
+    <t>Service Center Agent</t>
+  </si>
+  <si>
+    <t>Printing Supervisor</t>
+  </si>
+  <si>
+    <t>Printing User</t>
+  </si>
+  <si>
+    <t>Hamlah Owner</t>
+  </si>
+  <si>
+    <t>Hamlah User</t>
+  </si>
+  <si>
+    <t>Digital ID Issuer Supervisor</t>
+  </si>
+  <si>
+    <t>Digital ID Issuer</t>
+  </si>
+  <si>
+    <t>مشرف النظام</t>
+  </si>
+  <si>
+    <t>مستخدم النظام</t>
+  </si>
+  <si>
+    <t>مشرف التسجيل</t>
+  </si>
+  <si>
+    <t>موظف مركز الخدمة</t>
+  </si>
+  <si>
+    <t>مشرف الطباعة</t>
+  </si>
+  <si>
+    <t>موظف الطباعة</t>
+  </si>
+  <si>
+    <t>مشرف الحملة</t>
+  </si>
+  <si>
+    <t>موظف الحملة</t>
+  </si>
+  <si>
+    <t>مشرف المعرفات الرقمية</t>
+  </si>
+  <si>
+    <t>موظف المعرفات الرقمية</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -3016,7 +3109,7 @@
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3171,7 +3264,7 @@
         <v>239</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>210</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3182,7 +3275,7 @@
         <v>272</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>239</v>
@@ -3199,7 +3292,7 @@
         <v>273</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>239</v>
@@ -3216,7 +3309,7 @@
         <v>274</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>239</v>
@@ -3233,7 +3326,7 @@
         <v>281</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>239</v>
@@ -3250,7 +3343,7 @@
         <v>275</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>239</v>
@@ -3787,22 +3880,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="42.28515625" style="32" customWidth="1" collapsed="1"/>
-    <col min="4" max="8" width="9.140625" style="49"/>
+    <col min="2" max="5" width="42.28515625" style="32" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.140625" style="49"/>
     <col min="9" max="9" width="29.42578125" style="49" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="49"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>6</v>
       </c>
@@ -3812,8 +3905,14 @@
       <c r="C1" s="33" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="33" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -3823,8 +3922,14 @@
       <c r="C2" s="6" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -3834,8 +3939,14 @@
       <c r="C3" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>3</v>
       </c>
@@ -3845,8 +3956,14 @@
       <c r="C4" s="6" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>4</v>
       </c>
@@ -3856,8 +3973,14 @@
       <c r="C5" s="6" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D5" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>5</v>
       </c>
@@ -3867,8 +3990,14 @@
       <c r="C6" s="6" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>6</v>
       </c>
@@ -3878,8 +4007,14 @@
       <c r="C7" s="6" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26">
         <v>7</v>
       </c>
@@ -3889,8 +4024,14 @@
       <c r="C8" s="6" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>8</v>
       </c>
@@ -3900,8 +4041,14 @@
       <c r="C9" s="6" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
         <v>9</v>
       </c>
@@ -3911,8 +4058,14 @@
       <c r="C10" s="6" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26">
         <v>10</v>
       </c>
@@ -3922,8 +4075,14 @@
       <c r="C11" s="6" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>11</v>
       </c>
@@ -3933,8 +4092,14 @@
       <c r="C12" s="6" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <v>12</v>
       </c>
@@ -3944,8 +4109,14 @@
       <c r="C13" s="6" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>13</v>
       </c>
@@ -3956,7 +4127,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26">
         <v>14</v>
       </c>
@@ -3967,7 +4138,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26">
         <v>15</v>
       </c>
@@ -4118,10 +4289,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4138,12 +4309,14 @@
     <col min="11" max="11" width="18.85546875" style="32" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="15.85546875" style="32" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="11.42578125" style="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.42578125" style="32" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="18.140625" style="32" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="17.7109375" style="32" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="9.140625" style="30"/>
+    <col min="16" max="16" width="16.42578125" style="32" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.42578125" style="32" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
         <v>6</v>
       </c>
@@ -4189,8 +4362,14 @@
       <c r="O1" s="29" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="29" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26">
         <v>1</v>
       </c>
@@ -4231,13 +4410,19 @@
         <v>231</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>237</v>
+        <v>296</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q2" s="32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26">
         <v>2</v>
       </c>
@@ -4278,73 +4463,127 @@
         <v>279</v>
       </c>
       <c r="N3" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="O3" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="P3" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="O3" s="32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="6"/>
-    </row>
-    <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="32" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="G4" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="H4" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="K4" s="50" t="s">
+        <v>235</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>297</v>
+      </c>
+      <c r="O4" s="32" t="s">
+        <v>299</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="31"/>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="26"/>
       <c r="B6" s="31"/>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26"/>
       <c r="B7" s="31"/>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="31"/>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26"/>
       <c r="B9" s="31"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="31"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="31"/>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="31"/>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="31"/>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="31"/>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="31"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="31"/>
       <c r="C16" s="6"/>
@@ -4376,14 +4615,33 @@
   <hyperlinks>
     <hyperlink ref="K2" r:id="rId1"/>
     <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>RoleAuthorities!$E$2:$E$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>P2:Q1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>RoleAuthorities!$D$2:$D$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>N2:O1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
+<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4391,15 +4649,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4407,7 +4665,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -4419,25 +4677,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADE7FD43-B405-431A-BA03-1B7872428ECD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00EA3742-E182-4B0F-A945-862F886A2D8C}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: Printing Management : ValidateViewPrintingRequest
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -15,10 +15,11 @@
     <sheet name="UserRoles" sheetId="97" r:id="rId6"/>
     <sheet name="RoleAuthorities" sheetId="98" r:id="rId7"/>
     <sheet name="UserManagement" sheetId="81" r:id="rId8"/>
+    <sheet name="PrintingRequest" sheetId="99" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Driver!$A$1:$G$1</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="318">
   <si>
     <t>Execution_Flag</t>
   </si>
@@ -994,6 +995,21 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>ValidateViewPrintingRequest</t>
+  </si>
+  <si>
+    <t>Validate view Printing Request</t>
+  </si>
+  <si>
+    <t>RequestNumber</t>
+  </si>
+  <si>
+    <t>587220</t>
+  </si>
+  <si>
+    <t>PrintingRequest</t>
   </si>
 </sst>
 </file>
@@ -3102,14 +3118,14 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:CO13"/>
+  <dimension ref="A1:CO14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3258,7 +3274,7 @@
         <v>240</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>239</v>
@@ -3350,6 +3366,23 @@
       </c>
       <c r="E13" s="2" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -4640,8 +4673,147 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" style="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="42.85546875" style="32" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41.140625" style="32" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.42578125" style="32" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.140625" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="E1" s="29"/>
+    </row>
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="36"/>
+    </row>
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="26"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="26"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="26"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="26"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="6"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="26"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
+<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4649,15 +4821,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%HOSTNAME%">N12606.elm.com.sa</XMLData>
+<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4665,7 +4837,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -4677,25 +4849,25 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{828F99B3-A325-478D-A346-7ED3FDD66897}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00EA3742-E182-4B0F-A945-862F886A2D8C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C394F7-1EF4-44DC-811C-2AB6EF07FB23}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: Role Management : New UI updates
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -1582,7 +1582,68 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3125,7 +3186,7 @@
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3189,7 +3250,7 @@
         <v>208</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>103</v>
@@ -3203,10 +3264,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>103</v>
@@ -3220,10 +3281,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>103</v>
@@ -3237,10 +3298,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>103</v>
@@ -3257,7 +3318,7 @@
         <v>216</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>103</v>
@@ -3376,7 +3437,7 @@
         <v>313</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>317</v>
@@ -3386,56 +3447,80 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C27:C1048576">
-    <cfRule type="cellIs" dxfId="11" priority="33" operator="equal">
+  <conditionalFormatting sqref="C6:C1048576">
+    <cfRule type="cellIs" dxfId="17" priority="41" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="42" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F26:F1048576">
-    <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="cellIs" dxfId="15" priority="39" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="40" operator="equal">
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F25 C2:C26">
-    <cfRule type="containsText" dxfId="7" priority="29" operator="containsText" text="NO">
+  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
+    <cfRule type="containsText" dxfId="13" priority="37" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="30" operator="containsText" text="NO">
+    <cfRule type="containsText" dxfId="12" priority="38" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F25 C2:C26">
-    <cfRule type="containsText" dxfId="5" priority="27" operator="containsText" text="NO">
+  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
+    <cfRule type="containsText" dxfId="11" priority="35" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="28" operator="containsText" text="YES">
+    <cfRule type="containsText" dxfId="10" priority="36" operator="containsText" text="YES">
       <formula>NOT(ISERROR(SEARCH("YES",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C26">
-    <cfRule type="cellIs" dxfId="3" priority="14" operator="equal">
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
       <formula>"no"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F25">
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+  <conditionalFormatting sqref="C4:C5">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",C4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",C4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C5">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="NO">
+      <formula>NOT(ISERROR(SEARCH("NO",C4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="YES">
+      <formula>NOT(ISERROR(SEARCH("YES",C4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4:C5">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C6:C7">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"no"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 C2:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 F2:F1048576">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4867,7 +4952,7 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06C394F7-1EF4-44DC-811C-2AB6EF07FB23}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{344B711B-7D56-4464-A6AF-9CDFDCAD0593}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: User Management : New UI updates
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="317">
   <si>
     <t>Execution_Flag</t>
   </si>
@@ -992,9 +992,6 @@
   </si>
   <si>
     <t>موظف المعرفات الرقمية</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>ValidateViewPrintingRequest</t>
@@ -3186,7 +3183,7 @@
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3250,7 +3247,7 @@
         <v>208</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>103</v>
@@ -3267,7 +3264,7 @@
         <v>220</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>103</v>
@@ -3284,7 +3281,7 @@
         <v>215</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>103</v>
@@ -3301,7 +3298,7 @@
         <v>214</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>103</v>
@@ -3318,7 +3315,7 @@
         <v>216</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>103</v>
@@ -3335,13 +3332,13 @@
         <v>240</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>239</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>312</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3349,10 +3346,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>239</v>
@@ -3366,10 +3363,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>239</v>
@@ -3383,10 +3380,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>239</v>
@@ -3403,7 +3400,7 @@
         <v>281</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>239</v>
@@ -3420,7 +3417,7 @@
         <v>275</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>239</v>
@@ -3434,13 +3431,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>209</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>210</v>
@@ -3463,7 +3460,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
+  <conditionalFormatting sqref="C2:C3 C6:C26 F2:F25">
     <cfRule type="containsText" dxfId="13" priority="37" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
@@ -3471,7 +3468,7 @@
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
+  <conditionalFormatting sqref="C2:C3 C6:C26 F2:F25">
     <cfRule type="containsText" dxfId="11" priority="35" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
@@ -4410,7 +4407,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4787,7 +4784,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E1" s="29"/>
     </row>
@@ -4799,10 +4796,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4902,19 +4899,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">aelsayed</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%USERNAME%">aelsayed</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4928,31 +4925,31 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E7C6E9-F6DD-4B3D-8C39-8D90B603AEF5}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{344B711B-7D56-4464-A6AF-9CDFDCAD0593}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E089BE1D-D9FD-41FD-8B83-182DD70821F3}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-1 :: otp.component.html : add id attribute
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -3183,7 +3183,7 @@
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3349,7 +3349,7 @@
         <v>273</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D9" s="13" t="s">
         <v>239</v>
@@ -3366,7 +3366,7 @@
         <v>274</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>239</v>
@@ -3383,7 +3383,7 @@
         <v>272</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>239</v>
@@ -3400,7 +3400,7 @@
         <v>281</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>239</v>
@@ -3417,7 +3417,7 @@
         <v>275</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>12</v>
+        <v>209</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>239</v>
@@ -3460,7 +3460,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3 C6:C26 F2:F25">
+  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
     <cfRule type="containsText" dxfId="13" priority="37" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
@@ -3468,7 +3468,7 @@
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3 C6:C26 F2:F25">
+  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
     <cfRule type="containsText" dxfId="11" priority="35" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
@@ -3517,7 +3517,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576 F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 C2:C1048576">
       <formula1>"YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4899,19 +4899,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%USERNAME%">aelsayed</XMLData>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">aelsayed</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4925,31 +4925,31 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E7C6E9-F6DD-4B3D-8C39-8D90B603AEF5}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E7C6E9-F6DD-4B3D-8C39-8D90B603AEF5}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E089BE1D-D9FD-41FD-8B83-182DD70821F3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEE2A17A-F30F-4896-BBC3-9FF2E5672445}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
HAJ-2 :: Refactoring : Navigators : UserManagement : RoleManagement
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -511,9 +511,6 @@
     <t>ValidateSystemLogin</t>
   </si>
   <si>
-    <t>http://localhost:4200/#/login</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
@@ -545,9 +542,6 @@
   </si>
   <si>
     <t>sa.gov.moi.securityinform.qa</t>
-  </si>
-  <si>
-    <t>Smart_Haj</t>
   </si>
   <si>
     <r>
@@ -1007,6 +1001,12 @@
   </si>
   <si>
     <t>PrintingRequest</t>
+  </si>
+  <si>
+    <t>Shaaer</t>
+  </si>
+  <si>
+    <t>http://10.33.191.211:8080/shj-admin/#/login</t>
   </si>
 </sst>
 </file>
@@ -2565,8 +2565,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2610,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>171</v>
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>159</v>
+        <v>316</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2646,22 +2646,22 @@
         <v>59</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52"/>
       <c r="B9" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52"/>
       <c r="B10" s="14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>50</v>
@@ -2673,17 +2673,17 @@
         <v>41</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" s="41"/>
     </row>
     <row r="12" spans="1:15" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="52"/>
       <c r="B12" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="41"/>
     </row>
@@ -2695,7 +2695,7 @@
       <c r="C13" s="46"/>
       <c r="D13" s="41"/>
       <c r="H13" s="53" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I13" s="54"/>
       <c r="J13" s="54"/>
@@ -2775,7 +2775,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H18" s="56"/>
       <c r="I18" s="57"/>
@@ -2858,7 +2858,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H23" s="56"/>
       <c r="I23" s="57"/>
@@ -2952,7 +2952,7 @@
         <v>36</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22"/>
@@ -2969,7 +2969,7 @@
         <v>37</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22"/>
@@ -2986,7 +2986,7 @@
         <v>38</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22"/>
@@ -3003,7 +3003,7 @@
         <v>26</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H32" s="22"/>
       <c r="I32" s="22"/>
@@ -3020,7 +3020,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H33" s="22"/>
       <c r="I33" s="22"/>
@@ -3037,7 +3037,7 @@
         <v>24</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3178,12 +3178,12 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CO14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9:C14"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3230,13 +3230,13 @@
         <v>158</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3244,16 +3244,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>103</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3261,16 +3261,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>103</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3278,16 +3278,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>103</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3295,16 +3295,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>103</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3312,16 +3312,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>103</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3329,16 +3329,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3346,16 +3346,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3363,16 +3363,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3380,16 +3380,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3397,16 +3397,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3414,16 +3414,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -3431,20 +3431,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>209</v>
+        <v>12</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C6:C1048576">
+  <conditionalFormatting sqref="C8:C1048576">
     <cfRule type="cellIs" dxfId="17" priority="41" operator="equal">
       <formula>"no"</formula>
     </cfRule>
@@ -3460,7 +3460,7 @@
       <formula>"no"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
+  <conditionalFormatting sqref="F2:F25 C2:C26">
     <cfRule type="containsText" dxfId="13" priority="37" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
@@ -3468,7 +3468,7 @@
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3 F2:F25 C6:C26">
+  <conditionalFormatting sqref="F2:F25 C2:C26">
     <cfRule type="containsText" dxfId="11" priority="35" operator="containsText" text="NO">
       <formula>NOT(ISERROR(SEARCH("NO",C2)))</formula>
     </cfRule>
@@ -3476,43 +3476,11 @@
       <formula>NOT(ISERROR(SEARCH("YES",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C3">
+  <conditionalFormatting sqref="C2:C14">
     <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
       <formula>"no"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C5">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",C4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",C4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C5">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="NO">
-      <formula>NOT(ISERROR(SEARCH("NO",C4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="YES">
-      <formula>NOT(ISERROR(SEARCH("YES",C4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C4:C5">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6:C7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"no"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"yes"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3567,7 +3535,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="47" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>156</v>
@@ -3633,7 +3601,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C3" s="25" t="s">
         <v>157</v>
@@ -3828,16 +3796,16 @@
         <v>40</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E1" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>204</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>205</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3848,19 +3816,19 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3871,19 +3839,19 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G3" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4015,16 +3983,16 @@
         <v>6</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4032,16 +4000,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4049,16 +4017,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4066,16 +4034,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4083,16 +4051,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4100,16 +4068,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4117,16 +4085,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4134,16 +4102,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4151,16 +4119,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4168,16 +4136,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4185,16 +4153,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4202,16 +4170,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4219,16 +4187,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4236,10 +4204,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4247,10 +4215,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4258,10 +4226,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C16" s="32" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4269,10 +4237,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C17" s="32" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4280,10 +4248,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C18" s="32" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4291,10 +4259,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4302,10 +4270,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C20" s="32" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4313,10 +4281,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4324,10 +4292,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4335,10 +4303,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4346,10 +4314,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4357,10 +4325,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4368,10 +4336,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C26" s="32" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4379,10 +4347,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C27" s="32" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4390,10 +4358,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -4445,19 +4413,19 @@
         <v>98</v>
       </c>
       <c r="E1" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="H1" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="I1" s="29" t="s">
         <v>225</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>227</v>
       </c>
       <c r="J1" s="29" t="s">
         <v>99</v>
@@ -4472,16 +4440,16 @@
         <v>102</v>
       </c>
       <c r="N1" s="29" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="O1" s="29" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="Q1" s="29" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4492,49 +4460,49 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>62</v>
       </c>
       <c r="F2" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="G2" s="34" t="s">
-        <v>232</v>
-      </c>
-      <c r="H2" s="34" t="s">
+      <c r="J2" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="K2" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="L2" s="32" t="s">
         <v>234</v>
       </c>
-      <c r="J2" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="K2" s="50" t="s">
-        <v>235</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>236</v>
-      </c>
       <c r="M2" s="32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="N2" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="O2" s="32" t="s">
         <v>296</v>
       </c>
-      <c r="O2" s="32" t="s">
-        <v>298</v>
-      </c>
       <c r="P2" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q2" s="32" t="s">
         <v>306</v>
-      </c>
-      <c r="Q2" s="32" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4545,49 +4513,49 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>62</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H3" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="J3" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="K3" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="L3" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="M3" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="J3" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="K3" s="50" t="s">
+      <c r="N3" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="O3" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="P3" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="L3" s="32" t="s">
-        <v>278</v>
-      </c>
-      <c r="M3" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="O3" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="P3" s="32" t="s">
-        <v>237</v>
-      </c>
       <c r="Q3" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4598,49 +4566,49 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>62</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="H4" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="I4" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="K4" s="50" t="s">
         <v>233</v>
       </c>
-      <c r="I4" s="34" t="s">
-        <v>283</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="K4" s="50" t="s">
-        <v>235</v>
-      </c>
       <c r="L4" s="32" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M4" s="32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="N4" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="O4" s="32" t="s">
         <v>297</v>
       </c>
-      <c r="O4" s="32" t="s">
-        <v>299</v>
-      </c>
       <c r="P4" s="32" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q4" s="32" t="s">
         <v>307</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4784,7 +4752,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E1" s="29"/>
     </row>
@@ -4796,10 +4764,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>313</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4899,19 +4867,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%USERNAME%">aelsayed</XMLData>
+<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <XMLData TextToDisplay="%EMAILADDRESS%">aelsayed@elm.sa</XMLData>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%DOCUMENTGUID%">{00000000-0000-0000-0000-000000000000}</XMLData>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<XMLData TextToDisplay="%CLASSIFICATIONDATETIME%">15:27 07/04/2021</XMLData>
+<XMLData TextToDisplay="%USERNAME%">aelsayed</XMLData>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4925,25 +4893,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E7C6E9-F6DD-4B3D-8C39-8D90B603AEF5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C9B98AD0-472E-4815-AC1B-6688102EC9FA}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17DBF6F2-0BCB-43F2-A359-CBFCD8DDA352}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF29224A-3A23-4475-868F-2DEA160EE885}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11E7C6E9-F6DD-4B3D-8C39-8D90B603AEF5}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
HAJ-2 :: Enhancement : Navigators : UserManagement : RoleManagement
</commit_message>
<xml_diff>
--- a/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
+++ b/shj-admin-portal-automation/src/main/resources/test-assets/TestData/ControlFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4665" tabRatio="960" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="LookUp" sheetId="92" r:id="rId1"/>
@@ -880,9 +880,6 @@
     <t>ValidateDeleteUser</t>
   </si>
   <si>
-    <t>1010101012</t>
-  </si>
-  <si>
     <t>0551367732</t>
   </si>
   <si>
@@ -898,9 +895,6 @@
     <t>ValidateResetUserPassword</t>
   </si>
   <si>
-    <t>1010101013</t>
-  </si>
-  <si>
     <t>0551367733</t>
   </si>
   <si>
@@ -1007,6 +1001,12 @@
   </si>
   <si>
     <t>http://10.33.191.211:8080/shj-admin/#/login</t>
+  </si>
+  <si>
+    <t>1010101021</t>
+  </si>
+  <si>
+    <t>1010101022</t>
   </si>
 </sst>
 </file>
@@ -2565,8 +2565,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2610,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2628,7 +2628,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="43" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3183,7 +3183,7 @@
       <selection activeCell="C24" sqref="C24"/>
       <selection pane="topRight" activeCell="C24" sqref="C24"/>
       <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3247,7 +3247,7 @@
         <v>206</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>103</v>
@@ -3264,7 +3264,7 @@
         <v>218</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>103</v>
@@ -3281,7 +3281,7 @@
         <v>213</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>103</v>
@@ -3298,7 +3298,7 @@
         <v>212</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>103</v>
@@ -3315,7 +3315,7 @@
         <v>214</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>12</v>
+        <v>207</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>103</v>
@@ -3397,7 +3397,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>12</v>
@@ -3431,13 +3431,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C14" s="42" t="s">
         <v>12</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>208</v>
@@ -3989,10 +3989,10 @@
         <v>240</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4006,10 +4006,10 @@
         <v>241</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4023,10 +4023,10 @@
         <v>242</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4040,10 +4040,10 @@
         <v>243</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4057,7 +4057,7 @@
         <v>244</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>235</v>
@@ -4074,7 +4074,7 @@
         <v>245</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>236</v>
@@ -4091,10 +4091,10 @@
         <v>246</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4108,10 +4108,10 @@
         <v>247</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4125,10 +4125,10 @@
         <v>248</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4142,10 +4142,10 @@
         <v>249</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4159,10 +4159,10 @@
         <v>250</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4176,10 +4176,10 @@
         <v>251</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4193,10 +4193,10 @@
         <v>252</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4374,8 +4374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4446,10 +4446,10 @@
         <v>227</v>
       </c>
       <c r="P1" s="29" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="Q1" s="29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4463,7 +4463,7 @@
         <v>220</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="E2" s="34" t="s">
         <v>62</v>
@@ -4493,16 +4493,16 @@
         <v>229</v>
       </c>
       <c r="N2" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="O2" s="32" t="s">
         <v>294</v>
       </c>
-      <c r="O2" s="32" t="s">
-        <v>296</v>
-      </c>
       <c r="P2" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q2" s="32" t="s">
         <v>304</v>
-      </c>
-      <c r="Q2" s="32" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4513,10 +4513,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="E3" s="34" t="s">
         <v>62</v>
@@ -4531,7 +4531,7 @@
         <v>231</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J3" s="32" t="s">
         <v>228</v>
@@ -4540,22 +4540,22 @@
         <v>233</v>
       </c>
       <c r="L3" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="M3" s="32" t="s">
         <v>276</v>
       </c>
-      <c r="M3" s="32" t="s">
-        <v>277</v>
-      </c>
       <c r="N3" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="O3" s="32" t="s">
         <v>291</v>
-      </c>
-      <c r="O3" s="32" t="s">
-        <v>293</v>
       </c>
       <c r="P3" s="32" t="s">
         <v>235</v>
       </c>
       <c r="Q3" s="32" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4566,10 +4566,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>280</v>
+        <v>316</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>62</v>
@@ -4584,7 +4584,7 @@
         <v>231</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J4" s="32" t="s">
         <v>228</v>
@@ -4593,22 +4593,22 @@
         <v>233</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M4" s="32" t="s">
         <v>229</v>
       </c>
       <c r="N4" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="O4" s="32" t="s">
         <v>295</v>
       </c>
-      <c r="O4" s="32" t="s">
-        <v>297</v>
-      </c>
       <c r="P4" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q4" s="32" t="s">
         <v>305</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -4752,7 +4752,7 @@
         <v>40</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E1" s="29"/>
     </row>
@@ -4764,10 +4764,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" s="36" t="s">
         <v>311</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>